<commit_message>
Agregando nueva url para productos
</commit_message>
<xml_diff>
--- a/URL.xlsx
+++ b/URL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d64b28deae395d/Documentos/Krakedev/Módulo 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d64b28deae395d/Documentos/Krakedev/Módulo 3/Rest-West-Services-Inventario/Rest-West-Services-Inventario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EC1D479-FA22-4B36-97CD-73442F12DD41}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7F3335-AFBF-44C5-A27E-E1EC0B6DA8B9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
+    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>ACCION</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>Recupera todos los tipos de documentos</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/proveedores/crear</t>
+  </si>
+  <si>
+    <t>Crea un proveedor</t>
+  </si>
+  <si>
+    <t>/productos/buscar/{subcadena}</t>
+  </si>
+  <si>
+    <t>Recupera todos los productos cuyo nombre contenga la subcadena</t>
   </si>
 </sst>
 </file>
@@ -431,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1BA1DD-67D3-4550-A2A8-B456AF5C0685}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +491,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Url para registrar pedido
</commit_message>
<xml_diff>
--- a/URL.xlsx
+++ b/URL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d64b28deae395d/Documentos/Krakedev/Módulo 3/Rest-West-Services-Inventario/Rest-West-Services-Inventario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d64b28deae395d/Documentos/Krakedev/Módulo 3/Rest-West-Services-Inventario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C7F3335-AFBF-44C5-A27E-E1EC0B6DA8B9}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99831E7A-E9D2-41D8-8131-08CF19F7E428}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>ACCION</t>
   </si>
@@ -75,14 +75,34 @@
   </si>
   <si>
     <t>Recupera todos los productos cuyo nombre contenga la subcadena</t>
+  </si>
+  <si>
+    <t>/productos/crear</t>
+  </si>
+  <si>
+    <t>Crea un producto</t>
+  </si>
+  <si>
+    <t>/pedidos/registrar</t>
+  </si>
+  <si>
+    <t>Crea un pedido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -110,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1BA1DD-67D3-4550-A2A8-B456AF5C0685}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +534,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
URL put del método recibir pedido
</commit_message>
<xml_diff>
--- a/URL.xlsx
+++ b/URL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d64b28deae395d/Documentos/Krakedev/Módulo 3/Rest-West-Services-Inventario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99831E7A-E9D2-41D8-8131-08CF19F7E428}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BA2209F-8E35-4B6F-86A0-B25C37DA4C77}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
+    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ACCION</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Crea un pedido</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/pedidos/recibir</t>
+  </si>
+  <si>
+    <t>Recibe un pedido</t>
   </si>
 </sst>
 </file>
@@ -467,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1BA1DD-67D3-4550-A2A8-B456AF5C0685}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +565,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Insertando nuevas URLs de los servicios finales
</commit_message>
<xml_diff>
--- a/URL.xlsx
+++ b/URL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d64b28deae395d/Documentos/Krakedev/Módulo 3/Rest-West-Services-Inventario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66AD7EBD-B537-4112-90DC-9214479DEEF5}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{E5A4ED40-7291-46CC-8CC0-3110B306E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97860D5A-2AF2-4DE1-8488-8B6CE8CAFB40}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D540D84C-872E-4E3F-BA2E-40B71AB90A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>ACCION</t>
   </si>
@@ -102,6 +102,48 @@
   </si>
   <si>
     <t>Guarda las ventas</t>
+  </si>
+  <si>
+    <t>/productos/actualizar</t>
+  </si>
+  <si>
+    <t>Actualiza un producto</t>
+  </si>
+  <si>
+    <t>/categorias/crear</t>
+  </si>
+  <si>
+    <t>Crea una categoria</t>
+  </si>
+  <si>
+    <t>/categorias/actualizar</t>
+  </si>
+  <si>
+    <t>Actualiza una categoria</t>
+  </si>
+  <si>
+    <t>/categorias/probarRecuperar</t>
+  </si>
+  <si>
+    <t>Recupera todas las categorias</t>
+  </si>
+  <si>
+    <t>Recupera los pedidos con sus respectivos detalles de un determinado proveedor</t>
+  </si>
+  <si>
+    <t>Recupera el proveedor, recibiendo el id</t>
+  </si>
+  <si>
+    <t>/pedidos/buscarPorId{idProveedor}</t>
+  </si>
+  <si>
+    <t>/proveedores/buscarPorId/{idProveedor}</t>
+  </si>
+  <si>
+    <t>/productos/buscar/{codigo}</t>
+  </si>
+  <si>
+    <t>Recupera el producto, recbiendo el código</t>
   </si>
 </sst>
 </file>
@@ -486,16 +528,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1BA1DD-67D3-4550-A2A8-B456AF5C0685}">
-  <dimension ref="B2:D10"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="74.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -597,6 +639,83 @@
         <v>21</v>
       </c>
     </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>